<commit_message>
Fix #15617 - [Feature] Serving size labeled value for US
</commit_message>
<xml_diff>
--- a/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/en/ExportNutrients.xlsx
+++ b/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/en/ExportNutrients.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,15 +15,14 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">INCO!$A$3:$AL$3</definedName>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Nutrients!$B$3:$AL$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Nutrients!$B$3:$P$3</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Product!$A$3:$H$3</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">US!$A$3:$BA$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Nutrients!$B$3:$M$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Nutrients!$B$3:$AV$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Nutrients!$B$3:$AV$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Nutrients!$B$3:$AV$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Nutrients!$B$3:$AV$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Nutrients!$B$3:$AV$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Nutrients!$B$3:$AY$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Nutrients!$B$3:$AY$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Nutrients!$B$3:$AY$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Nutrients!$B$3:$AY$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Nutrients!$B$3:$AY$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="147">
   <si>
     <t xml:space="preserve">TYPE</t>
   </si>
@@ -112,6 +111,9 @@
     <t xml:space="preserve">bcpg:nutListValue</t>
   </si>
   <si>
+    <t xml:space="preserve">formula|T(fr.becpg.repo.product.formulation.nutrient.RegulationFormulationHelper).extractValue(props["prop_bcpg_nutListRoundedValue"],"EU")</t>
+  </si>
+  <si>
     <t xml:space="preserve">bcpg:nutListMini</t>
   </si>
   <si>
@@ -121,7 +123,10 @@
     <t xml:space="preserve">bcpg:nutListValuePerServing</t>
   </si>
   <si>
-    <t xml:space="preserve">bcpg:nutListGDAPerc</t>
+    <t xml:space="preserve">formula|T(fr.becpg.repo.product.formulation.nutrient.RegulationFormulationHelper).extractValuePerServing(props["prop_bcpg_nutListRoundedValue"],"EU")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">formula|T(fr.becpg.repo.product.formulation.nutrient.RegulationFormulationHelper).extractGDAPerc(props["prop_bcpg_nutListRoundedValue"],"EU")</t>
   </si>
   <si>
     <t xml:space="preserve">bcpg:nutListLossPerc</t>
@@ -139,6 +144,9 @@
     <t xml:space="preserve">Manual value</t>
   </si>
   <si>
+    <t xml:space="preserve">Labeled value EU</t>
+  </si>
+  <si>
     <t xml:space="preserve">Min</t>
   </si>
   <si>
@@ -148,7 +156,10 @@
     <t xml:space="preserve">1 serving</t>
   </si>
   <si>
-    <t xml:space="preserve">% GDA per serving</t>
+    <t xml:space="preserve">1 serving labeled EU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% GDA per serving (EU)</t>
   </si>
   <si>
     <t xml:space="preserve">% loss</t>
@@ -506,7 +517,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -540,6 +551,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -610,7 +626,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -639,15 +655,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -700,6 +720,29 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF004254"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -790,7 +833,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.98"/>
@@ -866,10 +909,10 @@
   <autoFilter ref="A3:H3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -881,13 +924,13 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BI3"/>
+  <dimension ref="A1:BL3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N11" activeCellId="0" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.72"/>
@@ -896,11 +939,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="17.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="21.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="12" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="6.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="21.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="13" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="6.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="6.21"/>
@@ -915,7 +956,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="33" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="6.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="93" min="38" style="0" width="6.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="6.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="39" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="96" min="41" style="0" width="6.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -968,8 +1011,11 @@
       <c r="AT1" s="1"/>
       <c r="AU1" s="1"/>
       <c r="AV1" s="1"/>
+      <c r="AW1" s="1"/>
+      <c r="AX1" s="1"/>
+      <c r="AY1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="67.15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
@@ -994,7 +1040,7 @@
       <c r="H2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="1" t="s">
         <v>25</v>
       </c>
       <c r="J2" s="6" t="s">
@@ -1006,12 +1052,16 @@
       <c r="L2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="6"/>
+      <c r="N2" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
+      <c r="P2" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
@@ -1057,50 +1107,57 @@
       <c r="BG2" s="6"/>
       <c r="BH2" s="6"/>
       <c r="BI2" s="6"/>
+      <c r="BJ2" s="6"/>
+      <c r="BK2" s="6"/>
+      <c r="BL2" s="6"/>
     </row>
-    <row r="3" s="11" customFormat="true" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7" t="s">
+    <row r="3" s="12" customFormat="true" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="F3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="G3" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="H3" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="I3" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="J3" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="K3" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
+      <c r="L3" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="Q3" s="6"/>
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
@@ -1133,12 +1190,15 @@
       <c r="AT3" s="6"/>
       <c r="AU3" s="6"/>
       <c r="AV3" s="6"/>
+      <c r="AW3" s="6"/>
+      <c r="AX3" s="6"/>
+      <c r="AY3" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="B3:AL3"/>
+  <autoFilter ref="B3:P3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1158,7 +1218,7 @@
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.98"/>
@@ -1294,139 +1354,139 @@
         <v>9</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="W2" s="6" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="Z2" s="6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="AB2" s="6" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AC2" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AD2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AI2" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="AE2" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AF2" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH2" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI2" s="6" t="s">
-        <v>56</v>
-      </c>
       <c r="AJ2" s="6" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AK2" s="6" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="AL2" s="6" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="AM2" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="AN2" s="6" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="AO2" s="6" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="AP2" s="6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="AQ2" s="6" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="AR2" s="6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="AS2" s="6" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="AT2" s="6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="AU2" s="6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="AV2" s="6" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AW2" s="6" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="AX2" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="AY2" s="6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AZ2" s="6" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="BA2" s="6" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="BB2" s="6"/>
       <c r="BC2" s="6"/>
@@ -1443,176 +1503,176 @@
       <c r="BN2" s="6"/>
       <c r="BO2" s="6"/>
     </row>
-    <row r="3" s="12" customFormat="true" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
+    <row r="3" s="13" customFormat="true" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="M3" s="10" t="s">
+      <c r="I3" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="J3" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="K3" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="L3" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="M3" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="R3" s="10" t="s">
+      <c r="N3" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="O3" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="T3" s="10" t="s">
+      <c r="P3" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="U3" s="10" t="s">
+      <c r="Q3" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="V3" s="10" t="s">
+      <c r="R3" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="W3" s="10" t="s">
+      <c r="S3" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="X3" s="10" t="s">
+      <c r="T3" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="Y3" s="10" t="s">
+      <c r="U3" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="Z3" s="10" t="s">
+      <c r="V3" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="AA3" s="10" t="s">
+      <c r="W3" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="AB3" s="10" t="s">
+      <c r="X3" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="AC3" s="10" t="s">
+      <c r="Y3" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="AD3" s="10" t="s">
+      <c r="Z3" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="AE3" s="10" t="s">
+      <c r="AA3" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="AF3" s="10" t="s">
+      <c r="AB3" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="AG3" s="10" t="s">
+      <c r="AC3" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="AH3" s="10" t="s">
+      <c r="AD3" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="AI3" s="10" t="s">
+      <c r="AE3" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="AJ3" s="10" t="s">
+      <c r="AF3" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="AK3" s="10" t="s">
+      <c r="AG3" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="AL3" s="10" t="s">
+      <c r="AH3" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="AM3" s="10" t="s">
+      <c r="AI3" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="AN3" s="10" t="s">
+      <c r="AJ3" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="AO3" s="10" t="s">
+      <c r="AK3" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="AP3" s="10" t="s">
+      <c r="AL3" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="AQ3" s="10" t="s">
+      <c r="AM3" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="AR3" s="10" t="s">
+      <c r="AN3" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="AS3" s="10" t="s">
+      <c r="AO3" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="AT3" s="10" t="s">
+      <c r="AP3" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="AU3" s="10" t="s">
+      <c r="AQ3" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="AV3" s="10" t="s">
+      <c r="AR3" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="AW3" s="10" t="s">
+      <c r="AS3" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="AX3" s="10" t="s">
+      <c r="AT3" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="AY3" s="10" t="s">
+      <c r="AU3" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="AZ3" s="10" t="s">
+      <c r="AV3" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="BA3" s="10" t="s">
+      <c r="AW3" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="BB3" s="14"/>
+      <c r="AX3" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="AY3" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="AZ3" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="BA3" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="BB3" s="15"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:BA3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1625,39 +1685,39 @@
   </sheetPr>
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="15" width="25.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="15" width="17.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="15" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="15" width="28.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="15" width="25.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="15" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="9" style="15" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="15" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="12" style="15" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="15" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="16" min="15" style="15" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="15" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="19" min="18" style="15" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="15" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="22" min="21" style="15" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="15" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="25" min="24" style="15" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="15" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="28" min="27" style="15" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="15" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="31" min="30" style="15" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="15" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="34" min="33" style="15" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="15" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="37" min="36" style="15" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="15" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="16" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="16" width="17.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="16" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="16" width="28.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="16" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="16" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="9" style="16" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="16" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="12" style="16" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="16" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="16" min="15" style="16" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="16" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="19" min="18" style="16" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="16" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="22" min="21" style="16" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="16" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="25" min="24" style="16" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="16" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="28" min="27" style="16" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="16" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="31" min="30" style="16" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="16" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="34" min="33" style="16" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="16" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="37" min="36" style="16" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="16" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="911" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -1665,394 +1725,394 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
-      <c r="W1" s="16"/>
-      <c r="X1" s="16"/>
-      <c r="Y1" s="16"/>
-      <c r="Z1" s="16"/>
-      <c r="AA1" s="16"/>
-      <c r="AB1" s="16"/>
-      <c r="AC1" s="16"/>
-      <c r="AD1" s="16"/>
-      <c r="AE1" s="16"/>
-      <c r="AF1" s="16"/>
-      <c r="AG1" s="16"/>
-      <c r="AH1" s="16"/>
-      <c r="AI1" s="16"/>
-      <c r="AJ1" s="16"/>
-      <c r="AK1" s="16"/>
-      <c r="AL1" s="16"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
+      <c r="AB1" s="17"/>
+      <c r="AC1" s="17"/>
+      <c r="AD1" s="17"/>
+      <c r="AE1" s="17"/>
+      <c r="AF1" s="17"/>
+      <c r="AG1" s="17"/>
+      <c r="AH1" s="17"/>
+      <c r="AI1" s="17"/>
+      <c r="AJ1" s="17"/>
+      <c r="AK1" s="17"/>
+      <c r="AL1" s="17"/>
     </row>
     <row r="2" customFormat="false" ht="57.45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="L2" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="M2" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="N2" s="17" t="s">
+      <c r="I2" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="O2" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="P2" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q2" s="17" t="s">
+      <c r="K2" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="P2" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="R2" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="S2" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="T2" s="17" t="s">
+      <c r="Q2" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="S2" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="U2" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="V2" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="W2" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="X2" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y2" s="17" t="s">
+      <c r="T2" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="U2" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="V2" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="W2" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="X2" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y2" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z2" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA2" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB2" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC2" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="AD2" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="Z2" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="AA2" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB2" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC2" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="AD2" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="AE2" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="AF2" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="AG2" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="AH2" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="AI2" s="17" t="s">
-        <v>131</v>
-      </c>
-      <c r="AJ2" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="AK2" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="AL2" s="17" t="s">
-        <v>67</v>
+      <c r="AE2" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF2" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG2" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="AH2" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI2" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="AJ2" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="AK2" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="AL2" s="18" t="s">
+        <v>71</v>
       </c>
     </row>
-    <row r="3" s="18" customFormat="true" ht="30.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18" t="s">
+    <row r="3" s="19" customFormat="true" ht="30.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="M3" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="P3" s="10" t="s">
+      <c r="I3" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="Q3" s="10" t="s">
+      <c r="J3" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="R3" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="S3" s="10" t="s">
+      <c r="K3" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="L3" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="T3" s="10" t="s">
+      <c r="M3" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="P3" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="U3" s="10" t="s">
+      <c r="Q3" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="T3" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="V3" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="W3" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="X3" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="Y3" s="10" t="s">
+      <c r="U3" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="V3" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="W3" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="X3" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y3" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z3" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA3" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="AB3" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="AC3" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="AD3" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="Z3" s="10" t="s">
+      <c r="AE3" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="AA3" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="AB3" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="AC3" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="AD3" s="10" t="s">
+      <c r="AF3" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="AG3" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="AH3" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="AI3" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="AE3" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="AF3" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="AG3" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="AH3" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="AI3" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="AJ3" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="AK3" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="AL3" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="AIA3" s="19"/>
-      <c r="AIB3" s="19"/>
-      <c r="AIC3" s="19"/>
-      <c r="AID3" s="19"/>
-      <c r="AIE3" s="19"/>
-      <c r="AIF3" s="19"/>
-      <c r="AIG3" s="19"/>
-      <c r="AIH3" s="19"/>
-      <c r="AII3" s="19"/>
-      <c r="AIJ3" s="19"/>
-      <c r="AIK3" s="19"/>
-      <c r="AIL3" s="19"/>
-      <c r="AIM3" s="19"/>
-      <c r="AIN3" s="19"/>
-      <c r="AIO3" s="19"/>
-      <c r="AIP3" s="19"/>
-      <c r="AIQ3" s="19"/>
-      <c r="AIR3" s="19"/>
-      <c r="AIS3" s="19"/>
-      <c r="AIT3" s="19"/>
-      <c r="AIU3" s="19"/>
-      <c r="AIV3" s="19"/>
-      <c r="AIW3" s="19"/>
-      <c r="AIX3" s="19"/>
-      <c r="AIY3" s="19"/>
-      <c r="AIZ3" s="19"/>
-      <c r="AJA3" s="19"/>
-      <c r="AJB3" s="19"/>
-      <c r="AJC3" s="19"/>
-      <c r="AJD3" s="19"/>
-      <c r="AJE3" s="19"/>
-      <c r="AJF3" s="19"/>
-      <c r="AJG3" s="19"/>
-      <c r="AJH3" s="19"/>
-      <c r="AJI3" s="19"/>
-      <c r="AJJ3" s="19"/>
-      <c r="AJK3" s="19"/>
-      <c r="AJL3" s="19"/>
-      <c r="AJM3" s="19"/>
-      <c r="AJN3" s="19"/>
-      <c r="AJO3" s="19"/>
-      <c r="AJP3" s="19"/>
-      <c r="AJQ3" s="19"/>
-      <c r="AJR3" s="19"/>
-      <c r="AJS3" s="19"/>
-      <c r="AJT3" s="19"/>
-      <c r="AJU3" s="19"/>
-      <c r="AJV3" s="19"/>
-      <c r="AJW3" s="19"/>
-      <c r="AJX3" s="19"/>
-      <c r="AJY3" s="19"/>
-      <c r="AJZ3" s="19"/>
-      <c r="AKA3" s="19"/>
-      <c r="AKB3" s="19"/>
-      <c r="AKC3" s="19"/>
-      <c r="AKD3" s="19"/>
-      <c r="AKE3" s="19"/>
-      <c r="AKF3" s="19"/>
-      <c r="AKG3" s="19"/>
-      <c r="AKH3" s="19"/>
-      <c r="AKI3" s="19"/>
-      <c r="AKJ3" s="19"/>
-      <c r="AKK3" s="19"/>
-      <c r="AKL3" s="19"/>
-      <c r="AKM3" s="19"/>
-      <c r="AKN3" s="19"/>
-      <c r="AKO3" s="19"/>
-      <c r="AKP3" s="19"/>
-      <c r="AKQ3" s="19"/>
-      <c r="AKR3" s="19"/>
-      <c r="AKS3" s="19"/>
-      <c r="AKT3" s="19"/>
-      <c r="AKU3" s="19"/>
-      <c r="AKV3" s="19"/>
-      <c r="AKW3" s="19"/>
-      <c r="AKX3" s="19"/>
-      <c r="AKY3" s="19"/>
-      <c r="AKZ3" s="19"/>
-      <c r="ALA3" s="19"/>
-      <c r="ALB3" s="19"/>
-      <c r="ALC3" s="19"/>
-      <c r="ALD3" s="19"/>
-      <c r="ALE3" s="19"/>
-      <c r="ALF3" s="19"/>
-      <c r="ALG3" s="19"/>
-      <c r="ALH3" s="19"/>
-      <c r="ALI3" s="19"/>
-      <c r="ALJ3" s="19"/>
-      <c r="ALK3" s="19"/>
-      <c r="ALL3" s="19"/>
-      <c r="ALM3" s="19"/>
-      <c r="ALN3" s="19"/>
-      <c r="ALO3" s="19"/>
-      <c r="ALP3" s="19"/>
-      <c r="ALQ3" s="19"/>
-      <c r="ALR3" s="19"/>
-      <c r="ALS3" s="19"/>
-      <c r="ALT3" s="19"/>
-      <c r="ALU3" s="19"/>
-      <c r="ALV3" s="19"/>
-      <c r="ALW3" s="19"/>
-      <c r="ALX3" s="19"/>
-      <c r="ALY3" s="19"/>
-      <c r="ALZ3" s="19"/>
-      <c r="AMA3" s="19"/>
-      <c r="AMB3" s="19"/>
-      <c r="AMC3" s="19"/>
-      <c r="AMD3" s="19"/>
-      <c r="AME3" s="19"/>
-      <c r="AMF3" s="19"/>
-      <c r="AMG3" s="19"/>
-      <c r="AMH3" s="19"/>
-      <c r="AMI3" s="19"/>
-      <c r="AMJ3" s="19"/>
+      <c r="AJ3" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="AK3" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="AL3" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="AIA3" s="20"/>
+      <c r="AIB3" s="20"/>
+      <c r="AIC3" s="20"/>
+      <c r="AID3" s="20"/>
+      <c r="AIE3" s="20"/>
+      <c r="AIF3" s="20"/>
+      <c r="AIG3" s="20"/>
+      <c r="AIH3" s="20"/>
+      <c r="AII3" s="20"/>
+      <c r="AIJ3" s="20"/>
+      <c r="AIK3" s="20"/>
+      <c r="AIL3" s="20"/>
+      <c r="AIM3" s="20"/>
+      <c r="AIN3" s="20"/>
+      <c r="AIO3" s="20"/>
+      <c r="AIP3" s="20"/>
+      <c r="AIQ3" s="20"/>
+      <c r="AIR3" s="20"/>
+      <c r="AIS3" s="20"/>
+      <c r="AIT3" s="20"/>
+      <c r="AIU3" s="20"/>
+      <c r="AIV3" s="20"/>
+      <c r="AIW3" s="20"/>
+      <c r="AIX3" s="20"/>
+      <c r="AIY3" s="20"/>
+      <c r="AIZ3" s="20"/>
+      <c r="AJA3" s="20"/>
+      <c r="AJB3" s="20"/>
+      <c r="AJC3" s="20"/>
+      <c r="AJD3" s="20"/>
+      <c r="AJE3" s="20"/>
+      <c r="AJF3" s="20"/>
+      <c r="AJG3" s="20"/>
+      <c r="AJH3" s="20"/>
+      <c r="AJI3" s="20"/>
+      <c r="AJJ3" s="20"/>
+      <c r="AJK3" s="20"/>
+      <c r="AJL3" s="20"/>
+      <c r="AJM3" s="20"/>
+      <c r="AJN3" s="20"/>
+      <c r="AJO3" s="20"/>
+      <c r="AJP3" s="20"/>
+      <c r="AJQ3" s="20"/>
+      <c r="AJR3" s="20"/>
+      <c r="AJS3" s="20"/>
+      <c r="AJT3" s="20"/>
+      <c r="AJU3" s="20"/>
+      <c r="AJV3" s="20"/>
+      <c r="AJW3" s="20"/>
+      <c r="AJX3" s="20"/>
+      <c r="AJY3" s="20"/>
+      <c r="AJZ3" s="20"/>
+      <c r="AKA3" s="20"/>
+      <c r="AKB3" s="20"/>
+      <c r="AKC3" s="20"/>
+      <c r="AKD3" s="20"/>
+      <c r="AKE3" s="20"/>
+      <c r="AKF3" s="20"/>
+      <c r="AKG3" s="20"/>
+      <c r="AKH3" s="20"/>
+      <c r="AKI3" s="20"/>
+      <c r="AKJ3" s="20"/>
+      <c r="AKK3" s="20"/>
+      <c r="AKL3" s="20"/>
+      <c r="AKM3" s="20"/>
+      <c r="AKN3" s="20"/>
+      <c r="AKO3" s="20"/>
+      <c r="AKP3" s="20"/>
+      <c r="AKQ3" s="20"/>
+      <c r="AKR3" s="20"/>
+      <c r="AKS3" s="20"/>
+      <c r="AKT3" s="20"/>
+      <c r="AKU3" s="20"/>
+      <c r="AKV3" s="20"/>
+      <c r="AKW3" s="20"/>
+      <c r="AKX3" s="20"/>
+      <c r="AKY3" s="20"/>
+      <c r="AKZ3" s="20"/>
+      <c r="ALA3" s="20"/>
+      <c r="ALB3" s="20"/>
+      <c r="ALC3" s="20"/>
+      <c r="ALD3" s="20"/>
+      <c r="ALE3" s="20"/>
+      <c r="ALF3" s="20"/>
+      <c r="ALG3" s="20"/>
+      <c r="ALH3" s="20"/>
+      <c r="ALI3" s="20"/>
+      <c r="ALJ3" s="20"/>
+      <c r="ALK3" s="20"/>
+      <c r="ALL3" s="20"/>
+      <c r="ALM3" s="20"/>
+      <c r="ALN3" s="20"/>
+      <c r="ALO3" s="20"/>
+      <c r="ALP3" s="20"/>
+      <c r="ALQ3" s="20"/>
+      <c r="ALR3" s="20"/>
+      <c r="ALS3" s="20"/>
+      <c r="ALT3" s="20"/>
+      <c r="ALU3" s="20"/>
+      <c r="ALV3" s="20"/>
+      <c r="ALW3" s="20"/>
+      <c r="ALX3" s="20"/>
+      <c r="ALY3" s="20"/>
+      <c r="ALZ3" s="20"/>
+      <c r="AMA3" s="20"/>
+      <c r="AMB3" s="20"/>
+      <c r="AMC3" s="20"/>
+      <c r="AMD3" s="20"/>
+      <c r="AME3" s="20"/>
+      <c r="AMF3" s="20"/>
+      <c r="AMG3" s="20"/>
+      <c r="AMH3" s="20"/>
+      <c r="AMI3" s="20"/>
+      <c r="AMJ3" s="20"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:AL3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix #18080 - [Feature] Add nutriscore in nutrient export
</commit_message>
<xml_diff>
--- a/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/en/ExportNutrients.xlsx
+++ b/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/en/ExportNutrients.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="151">
   <si>
     <t xml:space="preserve">TYPE</t>
   </si>
@@ -66,6 +66,12 @@
     <t xml:space="preserve">bcpg:legalName</t>
   </si>
   <si>
+    <t xml:space="preserve">bcpg:nutrientProfilingScore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:nutrientProfilingClass</t>
+  </si>
+  <si>
     <t xml:space="preserve">#</t>
   </si>
   <si>
@@ -88,6 +94,12 @@
   </si>
   <si>
     <t xml:space="preserve">Legal name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nutrient score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nutrient class</t>
   </si>
   <si>
     <t xml:space="preserve">bcpg:nutList</t>
@@ -517,7 +529,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -551,11 +563,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -626,7 +633,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -655,19 +662,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -827,13 +830,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.98"/>
@@ -843,9 +846,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="24.53"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -853,7 +858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
@@ -877,32 +882,44 @@
       </c>
       <c r="H2" s="2" t="s">
         <v>9</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -911,8 +928,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -926,11 +943,11 @@
   </sheetPr>
   <dimension ref="A1:BL3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N11" activeCellId="0" sqref="N11"/>
+    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.72"/>
@@ -966,7 +983,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1023,44 +1040,44 @@
         <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>30</v>
+        <v>33</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="O2" s="6"/>
       <c r="P2" s="6" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
@@ -1111,52 +1128,52 @@
       <c r="BK2" s="6"/>
       <c r="BL2" s="6"/>
     </row>
-    <row r="3" s="12" customFormat="true" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="9" t="s">
+    <row r="3" s="11" customFormat="true" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="B3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="I3" s="11" t="s">
+      <c r="E3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="H3" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="I3" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="J3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11" t="s">
+      <c r="K3" s="10" t="s">
         <v>42</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="Q3" s="6"/>
       <c r="R3" s="6"/>
@@ -1214,11 +1231,11 @@
   </sheetPr>
   <dimension ref="A1:BO3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.98"/>
@@ -1354,139 +1371,139 @@
         <v>9</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="W2" s="6" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="Z2" s="6" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="AB2" s="6" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="AC2" s="6" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="AD2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF2" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG2" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="AI2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="AE2" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF2" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="AG2" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="AH2" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AI2" s="6" t="s">
-        <v>60</v>
-      </c>
       <c r="AJ2" s="6" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="AK2" s="6" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="AL2" s="6" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="AM2" s="6" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="AN2" s="6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="AO2" s="6" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="AP2" s="6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="AQ2" s="6" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="AR2" s="6" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="AS2" s="6" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="AT2" s="6" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="AU2" s="6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="AV2" s="6" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="AW2" s="6" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="AX2" s="6" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="AY2" s="6" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="AZ2" s="6" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="BA2" s="6" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="BB2" s="6"/>
       <c r="BC2" s="6"/>
@@ -1503,167 +1520,167 @@
       <c r="BN2" s="6"/>
       <c r="BO2" s="6"/>
     </row>
-    <row r="3" s="13" customFormat="true" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="14" t="s">
+    <row r="3" s="12" customFormat="true" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="M3" s="11" t="s">
+      <c r="G3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="J3" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="K3" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="L3" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="M3" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="R3" s="11" t="s">
+      <c r="N3" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="S3" s="11" t="s">
+      <c r="O3" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="T3" s="11" t="s">
+      <c r="P3" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="U3" s="11" t="s">
+      <c r="Q3" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="V3" s="11" t="s">
+      <c r="R3" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="W3" s="11" t="s">
+      <c r="S3" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="X3" s="11" t="s">
+      <c r="T3" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="Y3" s="11" t="s">
+      <c r="U3" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="Z3" s="11" t="s">
+      <c r="V3" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="AA3" s="11" t="s">
+      <c r="W3" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="AB3" s="11" t="s">
+      <c r="X3" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="AC3" s="11" t="s">
+      <c r="Y3" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="AD3" s="11" t="s">
+      <c r="Z3" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="AE3" s="11" t="s">
+      <c r="AA3" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="AF3" s="11" t="s">
+      <c r="AB3" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="AG3" s="11" t="s">
+      <c r="AC3" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="AH3" s="11" t="s">
+      <c r="AD3" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="AI3" s="11" t="s">
+      <c r="AE3" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="AJ3" s="11" t="s">
+      <c r="AF3" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="AK3" s="11" t="s">
+      <c r="AG3" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="AL3" s="11" t="s">
+      <c r="AH3" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="AM3" s="11" t="s">
+      <c r="AI3" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="AN3" s="11" t="s">
+      <c r="AJ3" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="AO3" s="11" t="s">
+      <c r="AK3" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="AP3" s="11" t="s">
+      <c r="AL3" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="AQ3" s="11" t="s">
+      <c r="AM3" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="AR3" s="11" t="s">
+      <c r="AN3" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="AS3" s="11" t="s">
+      <c r="AO3" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="AT3" s="11" t="s">
+      <c r="AP3" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="AU3" s="11" t="s">
+      <c r="AQ3" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="AV3" s="11" t="s">
+      <c r="AR3" s="10" t="s">
         <v>126</v>
       </c>
-      <c r="AW3" s="11" t="s">
+      <c r="AS3" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="AX3" s="11" t="s">
+      <c r="AT3" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="AY3" s="11" t="s">
+      <c r="AU3" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="AZ3" s="11" t="s">
+      <c r="AV3" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="BA3" s="11" t="s">
+      <c r="AW3" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="BB3" s="15"/>
+      <c r="AX3" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="AY3" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="AZ3" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="BA3" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="BB3" s="14"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:BA3"/>
@@ -1671,8 +1688,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1685,39 +1702,39 @@
   </sheetPr>
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="16" width="25.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="16" width="17.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="16" width="20.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="16" width="28.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="16" width="25.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="16" width="26.13"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="9" style="16" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="16" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="12" style="16" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="16" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="16" min="15" style="16" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="16" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="19" min="18" style="16" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="16" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="22" min="21" style="16" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="16" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="25" min="24" style="16" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="16" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="28" min="27" style="16" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="16" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="31" min="30" style="16" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="16" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="34" min="33" style="16" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="16" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="37" min="36" style="16" width="19.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="16" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="15" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="15" width="17.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="15" width="20.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="15" width="28.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="15" width="25.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="15" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="9" style="15" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="15" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="13" min="12" style="15" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="15" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="16" min="15" style="15" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="15" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="19" min="18" style="15" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="15" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="22" min="21" style="15" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="15" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="25" min="24" style="15" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="15" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="28" min="27" style="15" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="15" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="31" min="30" style="15" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="15" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="34" min="33" style="15" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="15" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="37" min="36" style="15" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="15" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="911" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -1725,385 +1742,385 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17"/>
-      <c r="Y1" s="17"/>
-      <c r="Z1" s="17"/>
-      <c r="AA1" s="17"/>
-      <c r="AB1" s="17"/>
-      <c r="AC1" s="17"/>
-      <c r="AD1" s="17"/>
-      <c r="AE1" s="17"/>
-      <c r="AF1" s="17"/>
-      <c r="AG1" s="17"/>
-      <c r="AH1" s="17"/>
-      <c r="AI1" s="17"/>
-      <c r="AJ1" s="17"/>
-      <c r="AK1" s="17"/>
-      <c r="AL1" s="17"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
+      <c r="AG1" s="16"/>
+      <c r="AH1" s="16"/>
+      <c r="AI1" s="16"/>
+      <c r="AJ1" s="16"/>
+      <c r="AK1" s="16"/>
+      <c r="AL1" s="16"/>
     </row>
     <row r="2" customFormat="false" ht="57.45" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="J2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="K2" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="L2" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="N2" s="18" t="s">
+      <c r="I2" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="O2" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="P2" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q2" s="18" t="s">
+      <c r="K2" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="P2" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="R2" s="18" t="s">
-        <v>49</v>
-      </c>
-      <c r="S2" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="T2" s="18" t="s">
+      <c r="Q2" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="R2" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="S2" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="U2" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="V2" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="W2" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="X2" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y2" s="18" t="s">
+      <c r="T2" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="U2" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="V2" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="W2" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="X2" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y2" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z2" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA2" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="AB2" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="AC2" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="AD2" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="Z2" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA2" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="AB2" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="AC2" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="AD2" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="AE2" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF2" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="AG2" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="AH2" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="AI2" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="AJ2" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="AK2" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="AL2" s="18" t="s">
-        <v>71</v>
+      <c r="AE2" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF2" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG2" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="AH2" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="AI2" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="AJ2" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="AK2" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="AL2" s="17" t="s">
+        <v>75</v>
       </c>
     </row>
-    <row r="3" s="19" customFormat="true" ht="30.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="14" t="s">
+    <row r="3" s="18" customFormat="true" ht="30.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="P3" s="11" t="s">
+      <c r="G3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="J3" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="R3" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="S3" s="11" t="s">
+      <c r="K3" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="L3" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="T3" s="11" t="s">
+      <c r="M3" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="P3" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="U3" s="11" t="s">
+      <c r="Q3" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="T3" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="V3" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="W3" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="X3" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="Y3" s="11" t="s">
+      <c r="U3" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="V3" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="W3" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="X3" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y3" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z3" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA3" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="AB3" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="AC3" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="AD3" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="Z3" s="11" t="s">
+      <c r="AE3" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="AA3" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="AB3" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="AC3" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="AD3" s="11" t="s">
+      <c r="AF3" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="AG3" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="AH3" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI3" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="AE3" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="AF3" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="AG3" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="AH3" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="AI3" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="AJ3" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="AK3" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="AL3" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="AIA3" s="20"/>
-      <c r="AIB3" s="20"/>
-      <c r="AIC3" s="20"/>
-      <c r="AID3" s="20"/>
-      <c r="AIE3" s="20"/>
-      <c r="AIF3" s="20"/>
-      <c r="AIG3" s="20"/>
-      <c r="AIH3" s="20"/>
-      <c r="AII3" s="20"/>
-      <c r="AIJ3" s="20"/>
-      <c r="AIK3" s="20"/>
-      <c r="AIL3" s="20"/>
-      <c r="AIM3" s="20"/>
-      <c r="AIN3" s="20"/>
-      <c r="AIO3" s="20"/>
-      <c r="AIP3" s="20"/>
-      <c r="AIQ3" s="20"/>
-      <c r="AIR3" s="20"/>
-      <c r="AIS3" s="20"/>
-      <c r="AIT3" s="20"/>
-      <c r="AIU3" s="20"/>
-      <c r="AIV3" s="20"/>
-      <c r="AIW3" s="20"/>
-      <c r="AIX3" s="20"/>
-      <c r="AIY3" s="20"/>
-      <c r="AIZ3" s="20"/>
-      <c r="AJA3" s="20"/>
-      <c r="AJB3" s="20"/>
-      <c r="AJC3" s="20"/>
-      <c r="AJD3" s="20"/>
-      <c r="AJE3" s="20"/>
-      <c r="AJF3" s="20"/>
-      <c r="AJG3" s="20"/>
-      <c r="AJH3" s="20"/>
-      <c r="AJI3" s="20"/>
-      <c r="AJJ3" s="20"/>
-      <c r="AJK3" s="20"/>
-      <c r="AJL3" s="20"/>
-      <c r="AJM3" s="20"/>
-      <c r="AJN3" s="20"/>
-      <c r="AJO3" s="20"/>
-      <c r="AJP3" s="20"/>
-      <c r="AJQ3" s="20"/>
-      <c r="AJR3" s="20"/>
-      <c r="AJS3" s="20"/>
-      <c r="AJT3" s="20"/>
-      <c r="AJU3" s="20"/>
-      <c r="AJV3" s="20"/>
-      <c r="AJW3" s="20"/>
-      <c r="AJX3" s="20"/>
-      <c r="AJY3" s="20"/>
-      <c r="AJZ3" s="20"/>
-      <c r="AKA3" s="20"/>
-      <c r="AKB3" s="20"/>
-      <c r="AKC3" s="20"/>
-      <c r="AKD3" s="20"/>
-      <c r="AKE3" s="20"/>
-      <c r="AKF3" s="20"/>
-      <c r="AKG3" s="20"/>
-      <c r="AKH3" s="20"/>
-      <c r="AKI3" s="20"/>
-      <c r="AKJ3" s="20"/>
-      <c r="AKK3" s="20"/>
-      <c r="AKL3" s="20"/>
-      <c r="AKM3" s="20"/>
-      <c r="AKN3" s="20"/>
-      <c r="AKO3" s="20"/>
-      <c r="AKP3" s="20"/>
-      <c r="AKQ3" s="20"/>
-      <c r="AKR3" s="20"/>
-      <c r="AKS3" s="20"/>
-      <c r="AKT3" s="20"/>
-      <c r="AKU3" s="20"/>
-      <c r="AKV3" s="20"/>
-      <c r="AKW3" s="20"/>
-      <c r="AKX3" s="20"/>
-      <c r="AKY3" s="20"/>
-      <c r="AKZ3" s="20"/>
-      <c r="ALA3" s="20"/>
-      <c r="ALB3" s="20"/>
-      <c r="ALC3" s="20"/>
-      <c r="ALD3" s="20"/>
-      <c r="ALE3" s="20"/>
-      <c r="ALF3" s="20"/>
-      <c r="ALG3" s="20"/>
-      <c r="ALH3" s="20"/>
-      <c r="ALI3" s="20"/>
-      <c r="ALJ3" s="20"/>
-      <c r="ALK3" s="20"/>
-      <c r="ALL3" s="20"/>
-      <c r="ALM3" s="20"/>
-      <c r="ALN3" s="20"/>
-      <c r="ALO3" s="20"/>
-      <c r="ALP3" s="20"/>
-      <c r="ALQ3" s="20"/>
-      <c r="ALR3" s="20"/>
-      <c r="ALS3" s="20"/>
-      <c r="ALT3" s="20"/>
-      <c r="ALU3" s="20"/>
-      <c r="ALV3" s="20"/>
-      <c r="ALW3" s="20"/>
-      <c r="ALX3" s="20"/>
-      <c r="ALY3" s="20"/>
-      <c r="ALZ3" s="20"/>
-      <c r="AMA3" s="20"/>
-      <c r="AMB3" s="20"/>
-      <c r="AMC3" s="20"/>
-      <c r="AMD3" s="20"/>
-      <c r="AME3" s="20"/>
-      <c r="AMF3" s="20"/>
-      <c r="AMG3" s="20"/>
-      <c r="AMH3" s="20"/>
-      <c r="AMI3" s="20"/>
-      <c r="AMJ3" s="20"/>
+      <c r="AJ3" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="AK3" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="AL3" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="AIA3" s="19"/>
+      <c r="AIB3" s="19"/>
+      <c r="AIC3" s="19"/>
+      <c r="AID3" s="19"/>
+      <c r="AIE3" s="19"/>
+      <c r="AIF3" s="19"/>
+      <c r="AIG3" s="19"/>
+      <c r="AIH3" s="19"/>
+      <c r="AII3" s="19"/>
+      <c r="AIJ3" s="19"/>
+      <c r="AIK3" s="19"/>
+      <c r="AIL3" s="19"/>
+      <c r="AIM3" s="19"/>
+      <c r="AIN3" s="19"/>
+      <c r="AIO3" s="19"/>
+      <c r="AIP3" s="19"/>
+      <c r="AIQ3" s="19"/>
+      <c r="AIR3" s="19"/>
+      <c r="AIS3" s="19"/>
+      <c r="AIT3" s="19"/>
+      <c r="AIU3" s="19"/>
+      <c r="AIV3" s="19"/>
+      <c r="AIW3" s="19"/>
+      <c r="AIX3" s="19"/>
+      <c r="AIY3" s="19"/>
+      <c r="AIZ3" s="19"/>
+      <c r="AJA3" s="19"/>
+      <c r="AJB3" s="19"/>
+      <c r="AJC3" s="19"/>
+      <c r="AJD3" s="19"/>
+      <c r="AJE3" s="19"/>
+      <c r="AJF3" s="19"/>
+      <c r="AJG3" s="19"/>
+      <c r="AJH3" s="19"/>
+      <c r="AJI3" s="19"/>
+      <c r="AJJ3" s="19"/>
+      <c r="AJK3" s="19"/>
+      <c r="AJL3" s="19"/>
+      <c r="AJM3" s="19"/>
+      <c r="AJN3" s="19"/>
+      <c r="AJO3" s="19"/>
+      <c r="AJP3" s="19"/>
+      <c r="AJQ3" s="19"/>
+      <c r="AJR3" s="19"/>
+      <c r="AJS3" s="19"/>
+      <c r="AJT3" s="19"/>
+      <c r="AJU3" s="19"/>
+      <c r="AJV3" s="19"/>
+      <c r="AJW3" s="19"/>
+      <c r="AJX3" s="19"/>
+      <c r="AJY3" s="19"/>
+      <c r="AJZ3" s="19"/>
+      <c r="AKA3" s="19"/>
+      <c r="AKB3" s="19"/>
+      <c r="AKC3" s="19"/>
+      <c r="AKD3" s="19"/>
+      <c r="AKE3" s="19"/>
+      <c r="AKF3" s="19"/>
+      <c r="AKG3" s="19"/>
+      <c r="AKH3" s="19"/>
+      <c r="AKI3" s="19"/>
+      <c r="AKJ3" s="19"/>
+      <c r="AKK3" s="19"/>
+      <c r="AKL3" s="19"/>
+      <c r="AKM3" s="19"/>
+      <c r="AKN3" s="19"/>
+      <c r="AKO3" s="19"/>
+      <c r="AKP3" s="19"/>
+      <c r="AKQ3" s="19"/>
+      <c r="AKR3" s="19"/>
+      <c r="AKS3" s="19"/>
+      <c r="AKT3" s="19"/>
+      <c r="AKU3" s="19"/>
+      <c r="AKV3" s="19"/>
+      <c r="AKW3" s="19"/>
+      <c r="AKX3" s="19"/>
+      <c r="AKY3" s="19"/>
+      <c r="AKZ3" s="19"/>
+      <c r="ALA3" s="19"/>
+      <c r="ALB3" s="19"/>
+      <c r="ALC3" s="19"/>
+      <c r="ALD3" s="19"/>
+      <c r="ALE3" s="19"/>
+      <c r="ALF3" s="19"/>
+      <c r="ALG3" s="19"/>
+      <c r="ALH3" s="19"/>
+      <c r="ALI3" s="19"/>
+      <c r="ALJ3" s="19"/>
+      <c r="ALK3" s="19"/>
+      <c r="ALL3" s="19"/>
+      <c r="ALM3" s="19"/>
+      <c r="ALN3" s="19"/>
+      <c r="ALO3" s="19"/>
+      <c r="ALP3" s="19"/>
+      <c r="ALQ3" s="19"/>
+      <c r="ALR3" s="19"/>
+      <c r="ALS3" s="19"/>
+      <c r="ALT3" s="19"/>
+      <c r="ALU3" s="19"/>
+      <c r="ALV3" s="19"/>
+      <c r="ALW3" s="19"/>
+      <c r="ALX3" s="19"/>
+      <c r="ALY3" s="19"/>
+      <c r="ALZ3" s="19"/>
+      <c r="AMA3" s="19"/>
+      <c r="AMB3" s="19"/>
+      <c r="AMC3" s="19"/>
+      <c r="AMD3" s="19"/>
+      <c r="AME3" s="19"/>
+      <c r="AMF3" s="19"/>
+      <c r="AMG3" s="19"/>
+      <c r="AMH3" s="19"/>
+      <c r="AMI3" s="19"/>
+      <c r="AMJ3" s="19"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:AL3"/>
@@ -2111,8 +2128,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix #9722 - [Feature] Translate default search export
</commit_message>
<xml_diff>
--- a/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/en/ExportNutrients.xlsx
+++ b/becpg-plm/becpg-plm-core/src/main/resources/beCPG/birt/exportsearch/product/en/ExportNutrients.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,15 +14,19 @@
     <sheet name="INCO" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">INCO!$A$3:$AL$3</definedName>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Nutrients!$B$3:$P$3</definedName>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Product!$A$3:$H$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">INCO!$B$3:$AL$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Nutrients!$S$3:$T$3</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Product!$B$3:$P$3</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">US!$A$3:$BA$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Nutrients!$B$3:$AY$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Nutrients!$B$3:$AY$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Nutrients!$B$3:$AY$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Nutrients!$B$3:$AY$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Nutrients!$B$3:$AY$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Product!$A$3:$H$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Nutrients!$B$3:$AQ$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Nutrients!$B$3:$R$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Nutrients!$B$3:$BA$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Nutrients!$B$3:$BA$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Nutrients!$B$3:$BA$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Nutrients!$B$3:$BA$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Nutrients!$B$3:$BA$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">INCO!$A$3:$AL$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -34,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="173">
   <si>
     <t xml:space="preserve">TYPE</t>
   </si>
@@ -66,10 +70,28 @@
     <t xml:space="preserve">bcpg:legalName</t>
   </si>
   <si>
-    <t xml:space="preserve">bcpg:nutrientProfilingScore</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bcpg:nutrientProfilingClass</t>
+    <t xml:space="preserve">bcpg:servingSize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:servingSizeUnit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:servingSizeText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:numberOfServings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:nutrientPreparationState</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:nutrientPreparedUnit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:nutrientProfileCategory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:nutrientProfileVersion</t>
   </si>
   <si>
     <t xml:space="preserve">#</t>
@@ -96,10 +118,28 @@
     <t xml:space="preserve">Legal name</t>
   </si>
   <si>
-    <t xml:space="preserve">Nutrient score</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nutrient class</t>
+    <t xml:space="preserve">Serving size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serving size unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serving size text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of servings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nutritional value calculated for</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit of measure for as prepared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nutrient profile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nutrient profile version</t>
   </si>
   <si>
     <t xml:space="preserve">bcpg:nutList</t>
@@ -123,27 +163,42 @@
     <t xml:space="preserve">bcpg:nutListValue</t>
   </si>
   <si>
-    <t xml:space="preserve">formula|T(fr.becpg.repo.product.formulation.nutrient.RegulationFormulationHelper).extractValue(props["prop_bcpg_nutListRoundedValue"],"EU")</t>
+    <t xml:space="preserve">bcpg:nutListValuePrepared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:nutListFormulatedValuePrepared</t>
   </si>
   <si>
     <t xml:space="preserve">bcpg:nutListMini</t>
   </si>
   <si>
+    <t xml:space="preserve">bcpg:nutListFormulatedMini</t>
+  </si>
+  <si>
     <t xml:space="preserve">bcpg:nutListMaxi</t>
   </si>
   <si>
+    <t xml:space="preserve">bcpg:nutListFormulatedMaxi</t>
+  </si>
+  <si>
     <t xml:space="preserve">bcpg:nutListValuePerServing</t>
   </si>
   <si>
-    <t xml:space="preserve">formula|T(fr.becpg.repo.product.formulation.nutrient.RegulationFormulationHelper).extractValuePerServing(props["prop_bcpg_nutListRoundedValue"],"EU")</t>
-  </si>
-  <si>
-    <t xml:space="preserve">formula|T(fr.becpg.repo.product.formulation.nutrient.RegulationFormulationHelper).extractGDAPerc(props["prop_bcpg_nutListRoundedValue"],"EU")</t>
+    <t xml:space="preserve">bcpg:nutListFormulatedValuePerServing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:nutListGDAPerc</t>
   </si>
   <si>
     <t xml:space="preserve">bcpg:nutListLossPerc</t>
   </si>
   <si>
+    <t xml:space="preserve">bcpg:nutListMethod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bcpg:nutListMeasurementPrecision</t>
+  </si>
+  <si>
     <t xml:space="preserve">Variants</t>
   </si>
   <si>
@@ -156,25 +211,40 @@
     <t xml:space="preserve">Manual value</t>
   </si>
   <si>
-    <t xml:space="preserve">Labeled value EU</t>
+    <t xml:space="preserve">Value as prepared</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculated value as prepared</t>
   </si>
   <si>
     <t xml:space="preserve">Min</t>
   </si>
   <si>
+    <t xml:space="preserve">Formulated Min</t>
+  </si>
+  <si>
     <t xml:space="preserve">Max</t>
   </si>
   <si>
+    <t xml:space="preserve">Formulated Max</t>
+  </si>
+  <si>
     <t xml:space="preserve">1 serving</t>
   </si>
   <si>
-    <t xml:space="preserve">1 serving labeled EU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% GDA per serving (EU)</t>
+    <t xml:space="preserve">Calculated value per serving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% GDA per serving</t>
   </si>
   <si>
     <t xml:space="preserve">% loss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measurement precision</t>
   </si>
   <si>
     <t xml:space="preserve">bcpg:nutList[bcpg:nutListNut#gs1:nutrientTypeCode== "ENER-E14"]_bcpg:nutListFormulatedValue</t>
@@ -723,29 +793,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="00FFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF004254"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -830,10 +877,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P3" activeCellId="0" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -846,11 +893,18 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="28.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="19.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="24.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="18.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="20.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="31.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="32.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="24.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -858,7 +912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
@@ -888,45 +942,81 @@
       </c>
       <c r="J2" s="2" t="s">
         <v>11</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>21</v>
+        <v>27</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:H3"/>
+  <autoFilter ref="B3:P3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -941,10 +1031,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BL3"/>
+  <dimension ref="A1:BN3"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P3" activeCellId="0" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -956,26 +1046,33 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="26.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="17.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="21.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="13" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="6.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="6.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="21" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="6.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="24" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="6.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="27" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="6.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="30" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="6.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="33" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="6.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="36" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="6.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="39" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="96" min="41" style="0" width="6.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="15.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="21.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="13.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="23.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="6.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="23" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="6.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="26" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="6.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="6.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="32" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="6.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="35" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="6.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="38" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="6.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="41" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="98" min="43" style="0" width="6.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.2" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -983,7 +1080,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -1031,8 +1128,10 @@
       <c r="AW1" s="1"/>
       <c r="AX1" s="1"/>
       <c r="AY1" s="1"/>
+      <c r="AZ1" s="1"/>
+      <c r="BA1" s="1"/>
     </row>
-    <row r="2" customFormat="false" ht="67.15" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="46.25" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>2</v>
       </c>
@@ -1040,49 +1139,59 @@
         <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>33</v>
+        <v>44</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="O2" s="6"/>
+        <v>46</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>47</v>
+      </c>
       <c r="P2" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
+        <v>48</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
       <c r="W2" s="6"/>
@@ -1127,58 +1236,70 @@
       <c r="BJ2" s="6"/>
       <c r="BK2" s="6"/>
       <c r="BL2" s="6"/>
+      <c r="BM2" s="6"/>
+      <c r="BN2" s="6"/>
     </row>
     <row r="3" s="11" customFormat="true" ht="43.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="O3" s="10"/>
+        <v>62</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>63</v>
+      </c>
       <c r="P3" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
+        <v>64</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="T3" s="10" t="s">
+        <v>68</v>
+      </c>
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
       <c r="W3" s="6"/>
@@ -1210,12 +1331,14 @@
       <c r="AW3" s="6"/>
       <c r="AX3" s="6"/>
       <c r="AY3" s="6"/>
+      <c r="AZ3" s="6"/>
+      <c r="BA3" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="B3:P3"/>
+  <autoFilter ref="S3:T3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1231,7 +1354,7 @@
   </sheetPr>
   <dimension ref="A1:BO3"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -1371,139 +1494,139 @@
         <v>9</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="W2" s="6" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="Z2" s="6" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="AB2" s="6" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="AC2" s="6" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="AD2" s="6" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="AE2" s="6" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="AF2" s="6" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="AG2" s="6" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="AH2" s="6" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="AI2" s="6" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="AJ2" s="6" t="s">
-        <v>73</v>
+        <v>95</v>
       </c>
       <c r="AK2" s="6" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="AL2" s="6" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
       <c r="AM2" s="6" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="AN2" s="6" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="AO2" s="6" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="AP2" s="6" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="AQ2" s="6" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="AR2" s="6" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="AS2" s="6" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="AT2" s="6" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="AU2" s="6" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="AV2" s="6" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="AW2" s="6" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="AX2" s="6" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="AY2" s="6" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
       <c r="AZ2" s="6" t="s">
-        <v>89</v>
+        <v>111</v>
       </c>
       <c r="BA2" s="6" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="BB2" s="6"/>
       <c r="BC2" s="6"/>
@@ -1522,163 +1645,163 @@
     </row>
     <row r="3" s="12" customFormat="true" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>95</v>
+        <v>117</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="Q3" s="10" t="s">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="R3" s="10" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="T3" s="10" t="s">
-        <v>102</v>
+        <v>124</v>
       </c>
       <c r="U3" s="10" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="V3" s="10" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="W3" s="10" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="X3" s="10" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="Y3" s="10" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="Z3" s="10" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
       <c r="AA3" s="10" t="s">
-        <v>109</v>
+        <v>131</v>
       </c>
       <c r="AB3" s="10" t="s">
-        <v>110</v>
+        <v>132</v>
       </c>
       <c r="AC3" s="10" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
       <c r="AD3" s="10" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="AE3" s="10" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="AF3" s="10" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="AG3" s="10" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="AH3" s="10" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="AI3" s="10" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="AJ3" s="10" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="AK3" s="10" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="AL3" s="10" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
       <c r="AM3" s="10" t="s">
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="AN3" s="10" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="AO3" s="10" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="AP3" s="10" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
       <c r="AQ3" s="10" t="s">
-        <v>125</v>
+        <v>147</v>
       </c>
       <c r="AR3" s="10" t="s">
-        <v>126</v>
+        <v>148</v>
       </c>
       <c r="AS3" s="10" t="s">
-        <v>127</v>
+        <v>149</v>
       </c>
       <c r="AT3" s="10" t="s">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="AU3" s="10" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="AV3" s="10" t="s">
-        <v>130</v>
+        <v>152</v>
       </c>
       <c r="AW3" s="10" t="s">
-        <v>131</v>
+        <v>153</v>
       </c>
       <c r="AX3" s="10" t="s">
-        <v>132</v>
+        <v>154</v>
       </c>
       <c r="AY3" s="10" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="AZ3" s="10" t="s">
-        <v>134</v>
+        <v>156</v>
       </c>
       <c r="BA3" s="10" t="s">
-        <v>135</v>
+        <v>157</v>
       </c>
       <c r="BB3" s="14"/>
     </row>
@@ -1686,7 +1809,7 @@
   <autoFilter ref="A3:BA3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1702,8 +1825,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ3"/>
   <sheetViews>
-    <sheetView showFormulas="true" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1802,210 +1925,210 @@
         <v>9</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="L2" s="17" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>137</v>
+        <v>159</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="O2" s="17" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="Q2" s="17" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="R2" s="17" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="S2" s="17" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="T2" s="17" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="U2" s="17" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="V2" s="17" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="W2" s="17" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="X2" s="17" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="Y2" s="17" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="Z2" s="17" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="AA2" s="17" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="AB2" s="17" t="s">
-        <v>77</v>
+        <v>99</v>
       </c>
       <c r="AC2" s="17" t="s">
-        <v>138</v>
+        <v>160</v>
       </c>
       <c r="AD2" s="17" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="AE2" s="17" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="AF2" s="17" t="s">
-        <v>70</v>
+        <v>92</v>
       </c>
       <c r="AG2" s="17" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="AH2" s="17" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="AI2" s="17" t="s">
-        <v>139</v>
+        <v>161</v>
       </c>
       <c r="AJ2" s="17" t="s">
-        <v>140</v>
+        <v>162</v>
       </c>
       <c r="AK2" s="17" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c r="AL2" s="17" t="s">
-        <v>75</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" s="18" customFormat="true" ht="30.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>91</v>
+        <v>113</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>93</v>
+        <v>115</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="M3" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="T3" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="U3" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="V3" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="W3" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="X3" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y3" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="Z3" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA3" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="AB3" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="O3" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="P3" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q3" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="R3" s="10" t="s">
+      <c r="AC3" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="S3" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="T3" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="U3" s="10" t="s">
-        <v>103</v>
-      </c>
-      <c r="V3" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="W3" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="X3" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="Y3" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="Z3" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA3" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="AB3" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="AC3" s="10" t="s">
-        <v>123</v>
-      </c>
       <c r="AD3" s="10" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="AE3" s="10" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="AF3" s="10" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="AG3" s="10" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="AH3" s="10" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="AI3" s="10" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
       <c r="AJ3" s="10" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
       <c r="AK3" s="10" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="AL3" s="10" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
       <c r="AIA3" s="19"/>
       <c r="AIB3" s="19"/>
@@ -2123,10 +2246,10 @@
       <c r="AMJ3" s="19"/>
     </row>
   </sheetData>
-  <autoFilter ref="A3:AL3"/>
+  <autoFilter ref="B3:AL3"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>